<commit_message>
generate every knime dataDictionary for DATA_CLEANING subworkflows
</commit_message>
<xml_diff>
--- a/KNIME_nodes_MD4DSP_mapping.xlsx
+++ b/KNIME_nodes_MD4DSP_mapping.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
   <si>
     <t xml:space="preserve">No contemplado en nuestra librería</t>
   </si>
@@ -44,186 +44,6 @@
   </si>
   <si>
     <t xml:space="preserve">Missing Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number (double): Fix Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">imputeByFixValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number (double): Most Frequent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">imputeByDerivedValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number (double): Previous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number (double): Next</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number (double): Mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">imputeByNumericOp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number (double): Median</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number (double): Linear Interpolation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number (double): Closets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Row Filter (deprecated)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilter type: include rows by attribute value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilterRange/rowFilterPrimitive/rowFilterMissing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilter type: exclude rows by attribute value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilter type: include rows by number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilter type: exclude rows by number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilter type: include rows by rowID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilter type: exclude rows by rowID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">matching criteria: use pattern matching</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilterPrimitive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">matching criteria: use range checking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilterRange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">matching criteria: only missing values match</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilterMissing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column Filter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">included_columns --&gt; out_columns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">columnFilter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String to Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">categoricalToContinuous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numeric Outliers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sólo mappeado para la configuración - convertir todos los Outliers al valor permitido más cercano utilizando el cálculo de cuartil R_4 y el multiplicador de rango intercuartílico: 1.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numeric Binner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">binner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auto-Binner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Binning method: fixed number of bins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Binning method: Sample quantiles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bin_naming: numbered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bin naming: borders</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bin naming: midpoints</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Force integer bounds</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Math Formula</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Limitación de mapping - Sólo hecho para dos operandos (columnas o valores fijos) de operaciones SUMA, RESTA, MULTIPLICACIÓN y DIVISIÓN. El mapping del resto de operaciones mátemáticas queda para ser extendidas en el futuro, así como un número diferente de operandos.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mathOpFieldField / mathOpFieldFixValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Otras operaciones: '/', '*', 'log', 'exp',... con otros operadores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rule Engine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expression: $column_name$ LIKE "*fix_val*" =&gt; "fix_val"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mapping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expression: $column_name$ *operator* "num_operand" =&gt; "fix_val" siendo operator: &lt;, &lt;=, &gt;, &gt;=</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Otras expresiones con operadores: ? AND ?, ? IN ?, ? MATCHES ?, ? OR ?, ? XOR ?, FALSE, MISSING ?, NOT ?, TRUE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String Replacer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String Manipulation - String Manipulation (Multi Column)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Expresión con function: replace, replaceChars o substr. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Limitación para aplicarlo sobre una sóla columna de entrada</t>
-    </r>
   </si>
   <si>
     <r>
@@ -234,8 +54,24 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Functions: capitalize, removeChars, compare, count, countChars, indexOf, indexOfChars, join, joinStep, lastIndexOfChar, length, lowerCase, upperCase, md5Checksum, padLeft, padRight, regexMatcher, removeChars, removeDiacritic, removeDuplicates, regexReplace, removeUmlauts, reverse, string, strip, stripEnd, stripStart, toBoolean, toDouble, toInt, toLong, toNull, toEmpty, urlEncode, urlDecode. </t>
+      <t xml:space="preserve">Replacement type (String and Number): </t>
     </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Fix Value</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">imputeByFixValue</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -243,14 +79,378 @@
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Un ejemplo de función no mappeada es la función join($Name$, " - ", $City$)</t>
+      <t xml:space="preserve">Replacement type (String and Number): </t>
     </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Most Frequent</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">imputeByDerivedValue</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Replacement type (String and Number): </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Previous</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Replacement type (String and Number): </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Next</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Replacement type (Number): </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Maximum</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Replacement type (Number): </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Minimum</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">8/12 configuraciones mapeadas – 66%</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Replacement type (Number): </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Moving Average</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Replacement type (String): </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Remove Row</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Replacement type (Number): </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mean</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">imputeByNumericOp</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Replacement type (Number): </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Median</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Replacement type (Number): </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Linear Interpolation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Replacement type (Number): </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Closest</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Row Filter (deprecated)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilter type: include rows by attribute value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilterRange/rowFilterPrimitive/rowFilterMissing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilter type: exclude rows by attribute value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilter type: include rows by number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilter type: exclude rows by number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilter type: include rows by rowID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilter type: exclude rows by rowID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matching criteria: use pattern matching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilterPrimitive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matching criteria: use range checking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilterRange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">matching criteria: only missing values match</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilterMissing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column Filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">included_columns --&gt; out_columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">columnFilter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String to Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">categoricalToContinuous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numeric Outliers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sólo mappeado para la configuración - convertir todos los Outliers al valor permitido más cercano utilizando el cálculo de cuartil R_4 y el multiplicador de rango intercuartílico: 1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numeric Binner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">binner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto-Binner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binning method: fixed number of bins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binning method: Sample quantiles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bin_naming: numbered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bin naming: borders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bin naming: midpoints</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Force integer bounds</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Math Formula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limitación de mapping - Sólo hecho para dos operandos (columnas o valores fijos) de operaciones SUMA, RESTA, MULTIPLICACIÓN y DIVISIÓN. El mapping del resto de operaciones mátemáticas queda para ser extendidas en el futuro, así como un número diferente de operandos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mathOpFieldField / mathOpFieldFixValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otras operaciones: '/', '*', 'log', 'exp',... con otros operadores</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rule Engine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expression: $column_name$ LIKE "*fix_val*" =&gt; "fix_val"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mapping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expression: $column_name$ *operator* "num_operand" =&gt; "fix_val" siendo operator: &lt;, &lt;=, &gt;, &gt;=</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otras expresiones con operadores: ? AND ?, ? IN ?, ? MATCHES ?, ? OR ?, ? XOR ?, FALSE, MISSING ?, NOT ?, TRUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String Replacer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String Manipulation - String Manipulation (Multi Column)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expresión con function: replace, replaceChars o substr. Limitación para aplicarlo sobre una sóla columna de entrada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Functions: capitalize, removeChars, compare, count, countChars, indexOf, indexOfChars, join, joinStep, lastIndexOfChar, length, lowerCase, upperCase, md5Checksum, padLeft, padRight, regexMatcher, removeChars, removeDiacritic, removeDuplicates, regexReplace, removeUmlauts, reverse, string, strip, stripEnd, stripStart, toBoolean, toDouble, toInt, toLong, toNull, toEmpty, urlEncode, urlDecode. Un ejemplo de función no mappeada es la función join($Name$, " - ", $City$)</t>
   </si>
   <si>
     <t xml:space="preserve">Column Expressions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Expresión con function: replace, replaceChars o substr. Limitación para aplicarlo sobre una sóla columna de entrada</t>
   </si>
   <si>
     <t xml:space="preserve">Expresión matemática únicamente con dos operandos (columnas o valores fijos) de operaciones SUMA, RESTA, MULTIPLICACIÓN y DIVISIÓN. El mapping del resto de operaciones mátemáticas queda para ser extendidas en el futuro, así como un número diferente de operandos, así como ocurre en el mapeo de dichas operaciones para el nodo MathFormula</t>
@@ -266,7 +466,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -309,14 +509,41 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="JetBrains Mono"/>
-      <family val="0"/>
+      <family val="3"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="JetBrains Mono"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -332,18 +559,6 @@
       <name val="Aptos Narrow"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -413,7 +628,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -454,7 +669,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -462,7 +677,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -478,12 +701,32 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -491,54 +734,34 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -619,10 +842,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:M172"/>
+  <dimension ref="B1:M176"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C59" activeCellId="0" sqref="C59"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -710,7 +933,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="10"/>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="11" t="s">
@@ -723,7 +946,7 @@
     </row>
     <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="10"/>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="11" t="s">
@@ -734,9 +957,9 @@
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="10"/>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="12" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="11" t="s">
@@ -747,71 +970,77 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="10"/>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+    </row>
+    <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="10"/>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="10"/>
-      <c r="C12" s="8" t="s">
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+    </row>
+    <row r="12" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B12" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="C12" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="10"/>
-      <c r="C13" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="11" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-    </row>
-    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="14"/>
+      <c r="C14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>20</v>
+      <c r="B15" s="14"/>
+      <c r="C15" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="D15" s="11" t="s">
         <v>21</v>
@@ -822,9 +1051,9 @@
       <c r="H15" s="11"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="12"/>
-      <c r="C16" s="13" t="s">
-        <v>22</v>
+      <c r="B16" s="14"/>
+      <c r="C16" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="D16" s="11" t="s">
         <v>21</v>
@@ -835,137 +1064,138 @@
       <c r="H16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="12"/>
-      <c r="C17" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="15" t="s">
+      <c r="B17" s="14"/>
+      <c r="C17" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="12"/>
-      <c r="C18" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+    </row>
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="12"/>
-      <c r="C19" s="14" t="s">
+      <c r="B19" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
+      <c r="C19" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="12"/>
-      <c r="C20" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="15"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="12"/>
-      <c r="C21" s="13" t="s">
+      <c r="B21" s="10"/>
+      <c r="C21" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="12"/>
-      <c r="C22" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="11" t="s">
+      <c r="B22" s="10"/>
+      <c r="C22" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-    </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="12"/>
-      <c r="C23" s="13" t="s">
+      <c r="D22" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B23" s="10"/>
+      <c r="C23" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B24" s="10"/>
+      <c r="C24" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-    </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
+      <c r="D24" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="10"/>
+      <c r="C25" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="D25" s="11" t="s">
         <v>34</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>35</v>
       </c>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
       <c r="H25" s="11"/>
     </row>
-    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="17"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B27" s="16" t="s">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B26" s="10"/>
+      <c r="C26" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="14" t="s">
-        <v>34</v>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+    </row>
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B27" s="10"/>
+      <c r="C27" s="15" t="s">
+        <v>37</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
@@ -973,7 +1203,6 @@
       <c r="H27" s="11"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="14"/>
       <c r="C28" s="8"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
@@ -981,15 +1210,15 @@
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
     </row>
-    <row r="29" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B29" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
@@ -997,7 +1226,8 @@
       <c r="H29" s="11"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="14"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="8"/>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
@@ -1006,11 +1236,13 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B31" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="14"/>
       <c r="D31" s="11" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E31" s="11"/>
       <c r="F31" s="11"/>
@@ -1018,7 +1250,7 @@
       <c r="H31" s="11"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="13"/>
+      <c r="B32" s="16"/>
       <c r="C32" s="8"/>
       <c r="D32" s="9"/>
       <c r="E32" s="9"/>
@@ -1026,370 +1258,384 @@
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
     </row>
-    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>43</v>
+    <row r="33" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B33" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>45</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B34" s="19"/>
-      <c r="C34" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="13"/>
-    </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="19"/>
-      <c r="C35" s="13" t="s">
-        <v>45</v>
-      </c>
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="16"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B35" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="16"/>
       <c r="D35" s="11" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
-      <c r="I35" s="13"/>
-    </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="19"/>
-      <c r="C36" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="13"/>
+    </row>
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="15"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="19"/>
-      <c r="C37" s="13" t="s">
+      <c r="B37" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D37" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-      <c r="H37" s="15"/>
-      <c r="I37" s="13"/>
-    </row>
-    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="19"/>
-      <c r="C38" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-      <c r="H38" s="15"/>
-      <c r="I38" s="13"/>
-    </row>
-    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="13"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="13"/>
-    </row>
-    <row r="40" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="8" t="s">
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B38" s="21"/>
+      <c r="C38" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D38" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="15"/>
+    </row>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B39" s="21"/>
+      <c r="C39" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="13"/>
+      <c r="D39" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="15"/>
+    </row>
+    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B40" s="21"/>
+      <c r="C40" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="15"/>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="10"/>
-      <c r="C41" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D41" s="20" t="s">
+      <c r="B41" s="21"/>
+      <c r="C41" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="13"/>
-    </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D42" s="21"/>
-      <c r="E42" s="21"/>
-      <c r="F42" s="21"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="13"/>
-    </row>
-    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="12" t="s">
+      <c r="D41" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E41" s="17"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="15"/>
+    </row>
+    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B42" s="21"/>
+      <c r="C42" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="D42" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="15"/>
+    </row>
+    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="15"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="15"/>
+    </row>
+    <row r="44" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B44" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="C44" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="13"/>
-    </row>
-    <row r="44" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="12"/>
-      <c r="C44" s="8" t="s">
+      <c r="D44" s="11" t="s">
         <v>57</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>41</v>
       </c>
       <c r="E44" s="11"/>
       <c r="F44" s="11"/>
       <c r="G44" s="11"/>
       <c r="H44" s="11"/>
-      <c r="I44" s="13"/>
-    </row>
-    <row r="45" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="12"/>
+      <c r="I44" s="15"/>
+    </row>
+    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B45" s="22"/>
       <c r="C45" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D45" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="E45" s="22"/>
-      <c r="F45" s="22"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="22"/>
-      <c r="I45" s="13"/>
+      <c r="D45" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="15"/>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D46" s="21"/>
-      <c r="E46" s="21"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="13"/>
-    </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="23" t="s">
+      <c r="D46" s="23"/>
+      <c r="E46" s="23"/>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="15"/>
+    </row>
+    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B47" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C47" s="8"/>
+      <c r="C47" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="D47" s="11" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
-      <c r="I47" s="13"/>
-    </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C48" s="8"/>
-      <c r="D48" s="9"/>
-      <c r="E48" s="9"/>
-      <c r="F48" s="9"/>
-      <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="13"/>
-    </row>
-    <row r="49" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="C49" s="25" t="s">
+      <c r="I47" s="15"/>
+    </row>
+    <row r="48" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B48" s="10"/>
+      <c r="C48" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="15"/>
+    </row>
+    <row r="49" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B49" s="10"/>
+      <c r="C49" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" s="24"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
+      <c r="H49" s="24"/>
+      <c r="I49" s="15"/>
+    </row>
+    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D50" s="23"/>
+      <c r="E50" s="23"/>
+      <c r="F50" s="23"/>
+      <c r="G50" s="23"/>
+      <c r="H50" s="23"/>
+      <c r="I50" s="15"/>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B51" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C51" s="8"/>
+      <c r="D51" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D49" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="13"/>
-    </row>
-    <row r="50" customFormat="false" ht="68.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="24"/>
-      <c r="C50" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="D50" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="E50" s="22"/>
-      <c r="F50" s="22"/>
-      <c r="G50" s="22"/>
-      <c r="H50" s="22"/>
-      <c r="I50" s="13"/>
-    </row>
-    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I51" s="13"/>
-    </row>
-    <row r="52" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C52" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="13"/>
-    </row>
-    <row r="53" customFormat="false" ht="55.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="24"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="15"/>
+    </row>
+    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C52" s="8"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="15"/>
+    </row>
+    <row r="53" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B53" s="26" t="s">
+        <v>65</v>
+      </c>
       <c r="C53" s="27" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
       <c r="G53" s="11"/>
       <c r="H53" s="11"/>
-      <c r="I53" s="13"/>
-    </row>
-    <row r="54" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="24"/>
-      <c r="C54" s="27" t="s">
+      <c r="I53" s="15"/>
+    </row>
+    <row r="54" customFormat="false" ht="68.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B54" s="26"/>
+      <c r="C54" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D54" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" s="24"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="24"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="15"/>
+    </row>
+    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I55" s="15"/>
+    </row>
+    <row r="56" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B56" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="D54" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="E54" s="22"/>
-      <c r="F54" s="22"/>
-      <c r="G54" s="22"/>
-      <c r="H54" s="22"/>
-      <c r="I54" s="13"/>
-    </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="28"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="9"/>
-      <c r="F55" s="9"/>
-      <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="13"/>
-    </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="28"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="9"/>
-      <c r="F56" s="9"/>
-      <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="13"/>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="28"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="9"/>
-      <c r="F57" s="9"/>
-      <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="28"/>
-      <c r="C58" s="8"/>
-      <c r="D58" s="9"/>
-      <c r="E58" s="9"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
-      <c r="H58" s="9"/>
-    </row>
-    <row r="61" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C63" s="29"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9"/>
-      <c r="F63" s="9"/>
-      <c r="G63" s="9"/>
-      <c r="H63" s="9"/>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="28"/>
-      <c r="D64" s="9"/>
-      <c r="E64" s="9"/>
-      <c r="F64" s="9"/>
-      <c r="G64" s="9"/>
-      <c r="H64" s="9"/>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="28"/>
-      <c r="D65" s="9"/>
-      <c r="E65" s="9"/>
-      <c r="F65" s="9"/>
-      <c r="G65" s="9"/>
-      <c r="H65" s="9"/>
-    </row>
-    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D66" s="9"/>
-      <c r="E66" s="9"/>
-      <c r="F66" s="9"/>
-      <c r="G66" s="9"/>
-      <c r="H66" s="9"/>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="28"/>
+      <c r="D56" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="15"/>
+    </row>
+    <row r="57" customFormat="false" ht="55.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B57" s="26"/>
+      <c r="C57" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D57" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="15"/>
+    </row>
+    <row r="58" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B58" s="26"/>
+      <c r="C58" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="D58" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="15"/>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B59" s="30"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="15"/>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B60" s="30"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="15"/>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B61" s="30"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B62" s="30"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
+      <c r="H62" s="9"/>
+    </row>
+    <row r="65" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C67" s="31"/>
       <c r="D67" s="9"/>
       <c r="E67" s="9"/>
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
       <c r="H67" s="9"/>
     </row>
-    <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C68" s="8"/>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="30"/>
       <c r="D68" s="9"/>
       <c r="E68" s="9"/>
       <c r="F68" s="9"/>
@@ -1397,17 +1643,14 @@
       <c r="H68" s="9"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="28"/>
-      <c r="C69" s="8"/>
+      <c r="B69" s="30"/>
       <c r="D69" s="9"/>
       <c r="E69" s="9"/>
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
       <c r="H69" s="9"/>
     </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="28"/>
-      <c r="C70" s="8"/>
+    <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D70" s="9"/>
       <c r="E70" s="9"/>
       <c r="F70" s="9"/>
@@ -1416,15 +1659,13 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B71" s="30"/>
-      <c r="C71" s="8"/>
       <c r="D71" s="9"/>
       <c r="E71" s="9"/>
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
       <c r="H71" s="9"/>
     </row>
-    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="28"/>
+    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="8"/>
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
@@ -1433,7 +1674,7 @@
       <c r="H72" s="9"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="28"/>
+      <c r="B73" s="30"/>
       <c r="C73" s="8"/>
       <c r="D73" s="9"/>
       <c r="E73" s="9"/>
@@ -1442,7 +1683,7 @@
       <c r="H73" s="9"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="28"/>
+      <c r="B74" s="30"/>
       <c r="C74" s="8"/>
       <c r="D74" s="9"/>
       <c r="E74" s="9"/>
@@ -1451,7 +1692,7 @@
       <c r="H74" s="9"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="28"/>
+      <c r="B75" s="32"/>
       <c r="C75" s="8"/>
       <c r="D75" s="9"/>
       <c r="E75" s="9"/>
@@ -1469,7 +1710,7 @@
       <c r="H76" s="9"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="28"/>
+      <c r="B77" s="30"/>
       <c r="C77" s="8"/>
       <c r="D77" s="9"/>
       <c r="E77" s="9"/>
@@ -1478,7 +1719,7 @@
       <c r="H77" s="9"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="28"/>
+      <c r="B78" s="30"/>
       <c r="C78" s="8"/>
       <c r="D78" s="9"/>
       <c r="E78" s="9"/>
@@ -1487,8 +1728,8 @@
       <c r="H78" s="9"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="28"/>
-      <c r="C79" s="29"/>
+      <c r="B79" s="30"/>
+      <c r="C79" s="8"/>
       <c r="D79" s="9"/>
       <c r="E79" s="9"/>
       <c r="F79" s="9"/>
@@ -1496,8 +1737,8 @@
       <c r="H79" s="9"/>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="28"/>
-      <c r="C80" s="29"/>
+      <c r="B80" s="32"/>
+      <c r="C80" s="8"/>
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
       <c r="F80" s="9"/>
@@ -1505,8 +1746,8 @@
       <c r="H80" s="9"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="28"/>
-      <c r="C81" s="29"/>
+      <c r="B81" s="30"/>
+      <c r="C81" s="8"/>
       <c r="D81" s="9"/>
       <c r="E81" s="9"/>
       <c r="F81" s="9"/>
@@ -1514,8 +1755,8 @@
       <c r="H81" s="9"/>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="28"/>
-      <c r="C82" s="29"/>
+      <c r="B82" s="30"/>
+      <c r="C82" s="8"/>
       <c r="D82" s="9"/>
       <c r="E82" s="9"/>
       <c r="F82" s="9"/>
@@ -1523,8 +1764,8 @@
       <c r="H82" s="9"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="28"/>
-      <c r="C83" s="29"/>
+      <c r="B83" s="30"/>
+      <c r="C83" s="31"/>
       <c r="D83" s="9"/>
       <c r="E83" s="9"/>
       <c r="F83" s="9"/>
@@ -1532,8 +1773,8 @@
       <c r="H83" s="9"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="28"/>
-      <c r="C84" s="29"/>
+      <c r="B84" s="30"/>
+      <c r="C84" s="31"/>
       <c r="D84" s="9"/>
       <c r="E84" s="9"/>
       <c r="F84" s="9"/>
@@ -1541,7 +1782,8 @@
       <c r="H84" s="9"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="28"/>
+      <c r="B85" s="30"/>
+      <c r="C85" s="31"/>
       <c r="D85" s="9"/>
       <c r="E85" s="9"/>
       <c r="F85" s="9"/>
@@ -1549,7 +1791,8 @@
       <c r="H85" s="9"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="28"/>
+      <c r="B86" s="30"/>
+      <c r="C86" s="31"/>
       <c r="D86" s="9"/>
       <c r="E86" s="9"/>
       <c r="F86" s="9"/>
@@ -1557,7 +1800,8 @@
       <c r="H86" s="9"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="28"/>
+      <c r="B87" s="30"/>
+      <c r="C87" s="31"/>
       <c r="D87" s="9"/>
       <c r="E87" s="9"/>
       <c r="F87" s="9"/>
@@ -1565,7 +1809,8 @@
       <c r="H87" s="9"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="31"/>
+      <c r="B88" s="30"/>
+      <c r="C88" s="31"/>
       <c r="D88" s="9"/>
       <c r="E88" s="9"/>
       <c r="F88" s="9"/>
@@ -1573,7 +1818,7 @@
       <c r="H88" s="9"/>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="31"/>
+      <c r="B89" s="30"/>
       <c r="D89" s="9"/>
       <c r="E89" s="9"/>
       <c r="F89" s="9"/>
@@ -1581,7 +1826,7 @@
       <c r="H89" s="9"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="31"/>
+      <c r="B90" s="30"/>
       <c r="D90" s="9"/>
       <c r="E90" s="9"/>
       <c r="F90" s="9"/>
@@ -1589,7 +1834,7 @@
       <c r="H90" s="9"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="31"/>
+      <c r="B91" s="30"/>
       <c r="D91" s="9"/>
       <c r="E91" s="9"/>
       <c r="F91" s="9"/>
@@ -1597,7 +1842,7 @@
       <c r="H91" s="9"/>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="31"/>
+      <c r="B92" s="33"/>
       <c r="D92" s="9"/>
       <c r="E92" s="9"/>
       <c r="F92" s="9"/>
@@ -1605,7 +1850,7 @@
       <c r="H92" s="9"/>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="31"/>
+      <c r="B93" s="33"/>
       <c r="D93" s="9"/>
       <c r="E93" s="9"/>
       <c r="F93" s="9"/>
@@ -1613,7 +1858,7 @@
       <c r="H93" s="9"/>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="31"/>
+      <c r="B94" s="33"/>
       <c r="D94" s="9"/>
       <c r="E94" s="9"/>
       <c r="F94" s="9"/>
@@ -1621,7 +1866,7 @@
       <c r="H94" s="9"/>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="31"/>
+      <c r="B95" s="33"/>
       <c r="D95" s="9"/>
       <c r="E95" s="9"/>
       <c r="F95" s="9"/>
@@ -1629,7 +1874,7 @@
       <c r="H95" s="9"/>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="31"/>
+      <c r="B96" s="33"/>
       <c r="D96" s="9"/>
       <c r="E96" s="9"/>
       <c r="F96" s="9"/>
@@ -1637,7 +1882,7 @@
       <c r="H96" s="9"/>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="31"/>
+      <c r="B97" s="33"/>
       <c r="D97" s="9"/>
       <c r="E97" s="9"/>
       <c r="F97" s="9"/>
@@ -1645,35 +1890,39 @@
       <c r="H97" s="9"/>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="31"/>
+      <c r="B98" s="33"/>
       <c r="D98" s="9"/>
       <c r="E98" s="9"/>
       <c r="F98" s="9"/>
       <c r="G98" s="9"/>
       <c r="H98" s="9"/>
     </row>
-    <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B99" s="33"/>
       <c r="D99" s="9"/>
       <c r="E99" s="9"/>
       <c r="F99" s="9"/>
       <c r="G99" s="9"/>
       <c r="H99" s="9"/>
     </row>
-    <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B100" s="33"/>
       <c r="D100" s="9"/>
       <c r="E100" s="9"/>
       <c r="F100" s="9"/>
       <c r="G100" s="9"/>
       <c r="H100" s="9"/>
     </row>
-    <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B101" s="33"/>
       <c r="D101" s="9"/>
       <c r="E101" s="9"/>
       <c r="F101" s="9"/>
       <c r="G101" s="9"/>
       <c r="H101" s="9"/>
     </row>
-    <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B102" s="33"/>
       <c r="D102" s="9"/>
       <c r="E102" s="9"/>
       <c r="F102" s="9"/>
@@ -2170,8 +2419,36 @@
       <c r="G172" s="9"/>
       <c r="H172" s="9"/>
     </row>
+    <row r="173" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D173" s="9"/>
+      <c r="E173" s="9"/>
+      <c r="F173" s="9"/>
+      <c r="G173" s="9"/>
+      <c r="H173" s="9"/>
+    </row>
+    <row r="174" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D174" s="9"/>
+      <c r="E174" s="9"/>
+      <c r="F174" s="9"/>
+      <c r="G174" s="9"/>
+      <c r="H174" s="9"/>
+    </row>
+    <row r="175" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D175" s="9"/>
+      <c r="E175" s="9"/>
+      <c r="F175" s="9"/>
+      <c r="G175" s="9"/>
+      <c r="H175" s="9"/>
+    </row>
+    <row r="176" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D176" s="9"/>
+      <c r="E176" s="9"/>
+      <c r="F176" s="9"/>
+      <c r="G176" s="9"/>
+      <c r="H176" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="176">
+  <mergeCells count="181">
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:M2"/>
     <mergeCell ref="B3:H3"/>
@@ -2179,21 +2456,22 @@
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="D5:H5"/>
-    <mergeCell ref="B6:B13"/>
+    <mergeCell ref="B6:B11"/>
     <mergeCell ref="D6:H6"/>
     <mergeCell ref="D7:H7"/>
     <mergeCell ref="D8:H8"/>
     <mergeCell ref="D9:H9"/>
     <mergeCell ref="D10:H10"/>
     <mergeCell ref="D11:H11"/>
+    <mergeCell ref="B12:B17"/>
     <mergeCell ref="D12:H12"/>
     <mergeCell ref="D13:H13"/>
     <mergeCell ref="D14:H14"/>
-    <mergeCell ref="B15:B23"/>
     <mergeCell ref="D15:H15"/>
     <mergeCell ref="D16:H16"/>
     <mergeCell ref="D17:H17"/>
     <mergeCell ref="D18:H18"/>
+    <mergeCell ref="B19:B27"/>
     <mergeCell ref="D19:H19"/>
     <mergeCell ref="D20:H20"/>
     <mergeCell ref="D21:H21"/>
@@ -2208,40 +2486,40 @@
     <mergeCell ref="D30:H30"/>
     <mergeCell ref="D31:H31"/>
     <mergeCell ref="D32:H32"/>
-    <mergeCell ref="B33:B38"/>
     <mergeCell ref="D33:H33"/>
     <mergeCell ref="D34:H34"/>
     <mergeCell ref="D35:H35"/>
     <mergeCell ref="D36:H36"/>
+    <mergeCell ref="B37:B42"/>
     <mergeCell ref="D37:H37"/>
     <mergeCell ref="D38:H38"/>
     <mergeCell ref="D39:H39"/>
-    <mergeCell ref="B40:B41"/>
     <mergeCell ref="D40:H40"/>
     <mergeCell ref="D41:H41"/>
     <mergeCell ref="D42:H42"/>
-    <mergeCell ref="B43:B45"/>
     <mergeCell ref="D43:H43"/>
+    <mergeCell ref="B44:B45"/>
     <mergeCell ref="D44:H44"/>
     <mergeCell ref="D45:H45"/>
     <mergeCell ref="D46:H46"/>
+    <mergeCell ref="B47:B49"/>
     <mergeCell ref="D47:H47"/>
     <mergeCell ref="D48:H48"/>
-    <mergeCell ref="B49:B50"/>
     <mergeCell ref="D49:H49"/>
     <mergeCell ref="D50:H50"/>
-    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="D51:H51"/>
     <mergeCell ref="D52:H52"/>
+    <mergeCell ref="B53:B54"/>
     <mergeCell ref="D53:H53"/>
     <mergeCell ref="D54:H54"/>
-    <mergeCell ref="D55:H55"/>
+    <mergeCell ref="B56:B58"/>
     <mergeCell ref="D56:H56"/>
     <mergeCell ref="D57:H57"/>
     <mergeCell ref="D58:H58"/>
-    <mergeCell ref="D63:H63"/>
-    <mergeCell ref="D64:H64"/>
-    <mergeCell ref="D65:H65"/>
-    <mergeCell ref="D66:H66"/>
+    <mergeCell ref="D59:H59"/>
+    <mergeCell ref="D60:H60"/>
+    <mergeCell ref="D61:H61"/>
+    <mergeCell ref="D62:H62"/>
     <mergeCell ref="D67:H67"/>
     <mergeCell ref="D68:H68"/>
     <mergeCell ref="D69:H69"/>
@@ -2348,6 +2626,10 @@
     <mergeCell ref="D170:H170"/>
     <mergeCell ref="D171:H171"/>
     <mergeCell ref="D172:H172"/>
+    <mergeCell ref="D173:H173"/>
+    <mergeCell ref="D174:H174"/>
+    <mergeCell ref="D175:H175"/>
+    <mergeCell ref="D176:H176"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
updated knime node mapping relation
</commit_message>
<xml_diff>
--- a/KNIME_nodes_MD4DSP_mapping.xlsx
+++ b/KNIME_nodes_MD4DSP_mapping.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="89">
   <si>
     <t xml:space="preserve">No contemplado en nuestra librería</t>
   </si>
@@ -78,6 +78,7 @@
         <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Replacement type (String and Number): </t>
     </r>
@@ -103,6 +104,7 @@
         <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Replacement type (String and Number): </t>
     </r>
@@ -125,6 +127,7 @@
         <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Replacement type (String and Number): </t>
     </r>
@@ -135,6 +138,7 @@
         <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Next</t>
     </r>
@@ -146,6 +150,7 @@
         <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Replacement type (Number): </t>
     </r>
@@ -156,6 +161,7 @@
         <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Maximum</t>
     </r>
@@ -170,6 +176,7 @@
         <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Replacement type (Number): </t>
     </r>
@@ -180,11 +187,130 @@
         <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Minimum</t>
     </r>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Replacement type (Number): </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Moving Average</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Replacement type (String): </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Remove Row</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Replacement type (Number): </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Mean</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">imputeByNumericOp</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Replacement type (Number): </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Median</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Replacement type (Number): </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Linear Interpolation</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">8/12 configuraciones mapeadas – 66%</t>
   </si>
   <si>
@@ -194,6 +320,7 @@
         <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Replacement type (Number): </t>
     </r>
@@ -204,223 +331,217 @@
         <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Moving Average</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Replacement type (String): </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Remove Row</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Replacement type (Number): </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Mean</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">imputeByNumericOp</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Replacement type (Number): </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
+      <t xml:space="preserve">Closest</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Row Filter (deprecated)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Median</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Replacement type (Number): </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
+      <t xml:space="preserve">rowFilter type: include rows by attribute value | </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">matching criteria: use pattern matching</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilterPrimitive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilter type: include rows by attribute value | matching criteria: use range checking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilterRange</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilter type: include rows by attribute value | matching criteria: only missing values match</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilterMissing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilter type: exclude rows by attribute value | matching criteria: use pattern matching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilter type: exclude rows by attribute value | matching criteria: use range checking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilter type: exclude rows by attribute value | matching criteria: only missing values match</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilter type: include rows by number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilter type: exclude rows by number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilter type: include rows by rowID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6/10  configuraciones mapeadas – 60%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rowFilter type: exclude rows by rowID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Column Filter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">included_columns --&gt; out_columns | Column filter option: Manual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">columnFilter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">included_columns --&gt; out_columns | Column filter option: Wildcard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">included_columns --&gt; out_columns | Column filter option: Regex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¼ configuraciones mapeadas – 25%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">included_columns --&gt; out_columns | Column filter option: Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String to Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">categoricalToContinuous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/3 configuraciones mapeadas – 33%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numeric Outliers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sólo mappeado para la configuración - convertir todos los Outliers al valor permitido más cercano utilizando el cálculo de cuartil R_4 y el multiplicador de rango intercuartílico: 1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">configuraciones mapeadas – SIN DETERMINAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resto de configuraciones relativas a los parámetros: Interquartile range multiplier (k), quartile calculation, Oulier treatment: apply to., treatment option, replacement strategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numeric Binner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">binner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/1 configuraciones mapeadas – 100%%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Auto-Binner</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Linear Interpolation</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Replacement type (Number): </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
+      <t xml:space="preserve">Binning method: fixed number of bins | </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Bin_naming: numbered</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Aptos Narrow"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Closest</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Row Filter (deprecated)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilter type: include rows by attribute value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilterRange/rowFilterPrimitive/rowFilterMissing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilter type: exclude rows by attribute value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilter type: include rows by number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilter type: exclude rows by number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilter type: include rows by rowID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilter type: exclude rows by rowID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">matching criteria: use pattern matching</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilterPrimitive</t>
-  </si>
-  <si>
-    <t xml:space="preserve">matching criteria: use range checking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilterRange</t>
-  </si>
-  <si>
-    <t xml:space="preserve">matching criteria: only missing values match</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilterMissing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Column Filter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">included_columns --&gt; out_columns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">columnFilter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">String to Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">categoricalToContinuous</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numeric Outliers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sólo mappeado para la configuración - convertir todos los Outliers al valor permitido más cercano utilizando el cálculo de cuartil R_4 y el multiplicador de rango intercuartílico: 1.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numeric Binner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">binner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Auto-Binner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Binning method: fixed number of bins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Binning method: Sample quantiles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bin_naming: numbered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bin naming: borders</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bin naming: midpoints</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Force integer bounds</t>
+      <t xml:space="preserve">Binning method: Sample quantiles </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">| Bin_naming: numbered</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Binning method: fixed number of bins | </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Bin_naming: borders</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Binning method: Sample quantiles | Bin_naming: borders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binning method: fixed number of bins | Bin_naming: midpoints</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1/6 configuraciones mapeadas – 16%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binning method: Sample quantiles | Bin_naming: midpoints</t>
   </si>
   <si>
     <t xml:space="preserve">Math Formula</t>
   </si>
   <si>
-    <t xml:space="preserve">Limitación de mapping - Sólo hecho para dos operandos (columnas o valores fijos) de operaciones SUMA, RESTA, MULTIPLICACIÓN y DIVISIÓN. El mapping del resto de operaciones mátemáticas queda para ser extendidas en el futuro, así como un número diferente de operandos.</t>
+    <t xml:space="preserve">Limitación de mapping - Sólo hecho para dos operandos (columnas o valores fijos) de operaciones SUMA, RESTA, MULTIPLICACIÓN y DIVISIÓN. El mapping del resto de operaciones mátemáticas queda para ser extendidas en el futuro, así como un número diferente de operandos. Mapeo actual: caso base con 2 operandos y 1 operador.</t>
   </si>
   <si>
     <t xml:space="preserve">mathOpFieldField / mathOpFieldFixValue</t>
   </si>
   <si>
-    <t xml:space="preserve">Otras operaciones: '/', '*', 'log', 'exp',... con otros operadores</t>
+    <t xml:space="preserve">4/71 configuraciones mapeadas – 5.63%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otras operaciones: 'log', 'exp', sen(x), cos(x), tan(x),… con múltiples operadores y operandos (caso general)</t>
   </si>
   <si>
     <t xml:space="preserve">Rule Engine</t>
@@ -435,25 +556,46 @@
     <t xml:space="preserve">expression: $column_name$ *operator* "num_operand" =&gt; "fix_val" siendo operator: &lt;, &lt;=, &gt;, &gt;=</t>
   </si>
   <si>
-    <t xml:space="preserve">Otras expresiones con operadores: ? AND ?, ? IN ?, ? MATCHES ?, ? OR ?, ? XOR ?, FALSE, MISSING ?, NOT ?, TRUE</t>
+    <t xml:space="preserve">5/16 configuraciones mapeadas – 31.25%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Otras expresiones con operadores: ? AND ?, ? IN ?, ? MATCHES ?, ? OR ?, ? XOR ?, FALSE, MISSING ?, NOT ?, TRUE o expresiones más complejas</t>
   </si>
   <si>
     <t xml:space="preserve">String Replacer</t>
   </si>
   <si>
+    <t xml:space="preserve">Patern – Replacement text | Replacement type: Literal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patern – Replacement text | Replacement type: Wildcard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">⅓ configuraciones mapeadas – 33%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patern – Replacement text | Replacement type: Regex</t>
+  </si>
+  <si>
     <t xml:space="preserve">String Manipulation - String Manipulation (Multi Column)</t>
   </si>
   <si>
     <t xml:space="preserve">Expresión con function: replace, replaceChars o substr. Limitación para aplicarlo sobre una sóla columna de entrada</t>
   </si>
   <si>
-    <t xml:space="preserve">Functions: capitalize, removeChars, compare, count, countChars, indexOf, indexOfChars, join, joinStep, lastIndexOfChar, length, lowerCase, upperCase, md5Checksum, padLeft, padRight, regexMatcher, removeChars, removeDiacritic, removeDuplicates, regexReplace, removeUmlauts, reverse, string, strip, stripEnd, stripStart, toBoolean, toDouble, toInt, toLong, toNull, toEmpty, urlEncode, urlDecode. Un ejemplo de función no mappeada es la función join($Name$, " - ", $City$)</t>
+    <t xml:space="preserve">3/53 configuraciones mapeadas – 5.6%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Functions: capitalize, removeChars, compare, count, countChars, indexOf, indexOfChars, join, joinStep, lastIndexOfChar, length, lowerCase, upperCase, md5Checksum, padLeft, padRight, regexMatcher, removeChars, removeDiacritic, removeDuplicates, regexReplace, removeUmlauts, reverse, string, strip, stripEnd, stripStart, toBoolean, toDouble, toInt, toLong, toNull, toEmpty, urlEncode, urlDecode. Tampoco es posible mappear funciones anidadas. Un ejemplo de función no mappeada es la función join($Name$, " - ", $City$)</t>
   </si>
   <si>
     <t xml:space="preserve">Column Expressions</t>
   </si>
   <si>
     <t xml:space="preserve">Expresión matemática únicamente con dos operandos (columnas o valores fijos) de operaciones SUMA, RESTA, MULTIPLICACIÓN y DIVISIÓN. El mapping del resto de operaciones mátemáticas queda para ser extendidas en el futuro, así como un número diferente de operandos, así como ocurre en el mapeo de dichas operaciones para el nodo MathFormula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7/185 configuraciones mapeadas – 3.78%</t>
   </si>
   <si>
     <t xml:space="preserve">Resto de funciones de manipulación de strings, operaciones matemáticas, HTML, accesos, operaciones lógicas o de manipulación del path. Un ejemplo de función de manipulación de strings no mappeada es la función join($Name$, " - ", $City$)</t>
@@ -463,10 +605,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -521,23 +664,16 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
     </font>
     <font>
       <sz val="12"/>
@@ -628,7 +764,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -677,7 +813,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -685,83 +821,103 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -842,16 +998,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:M176"/>
+  <dimension ref="B1:M186"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="D68" activeCellId="0" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="96.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="55.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="99.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.11"/>
   </cols>
@@ -997,11 +1153,9 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="10"/>
+      <c r="C12" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>15</v>
@@ -1012,9 +1166,9 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="14"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>15</v>
@@ -1025,12 +1179,12 @@
       <c r="H13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="14"/>
+      <c r="B14" s="10"/>
       <c r="C14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="11" t="s">
         <v>20</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>21</v>
       </c>
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
@@ -1038,12 +1192,12 @@
       <c r="H14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="14"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
@@ -1051,12 +1205,12 @@
       <c r="H15" s="11"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="14"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16" s="11"/>
       <c r="F16" s="11"/>
@@ -1064,12 +1218,14 @@
       <c r="H16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="14"/>
+      <c r="B17" s="14" t="s">
+        <v>23</v>
+      </c>
       <c r="C17" s="12" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
@@ -1090,21 +1246,21 @@
       <c r="C19" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="10"/>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="17" t="s">
         <v>28</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="11"/>
@@ -1113,168 +1269,177 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="10"/>
-      <c r="C21" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
+      <c r="C21" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="10"/>
-      <c r="C22" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="17" t="s">
+      <c r="C22" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="10"/>
-      <c r="C23" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
+      <c r="C23" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="10"/>
-      <c r="C24" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
+      <c r="C24" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="10"/>
-      <c r="C25" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
+      <c r="C25" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="10"/>
-      <c r="C26" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D26" s="11" t="s">
+      <c r="C26" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-    </row>
-    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D26" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="10"/>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B28" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-    </row>
-    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C28" s="8"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="18" t="s">
+      <c r="C28" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="D28" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+    </row>
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C29" s="8"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B30" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="C30" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-    </row>
-    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="19"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="9"/>
-      <c r="E30" s="9"/>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
+      <c r="D30" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="D31" s="11" t="s">
+      <c r="B31" s="19"/>
+      <c r="C31" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-    </row>
-    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="16"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-    </row>
-    <row r="33" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="20" t="s">
+      <c r="D31" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B32" s="19"/>
+      <c r="C32" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="D32" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B33" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-    </row>
-    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="16"/>
+      <c r="C33" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="22"/>
+      <c r="C34" s="8"/>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
       <c r="F34" s="9"/>
@@ -1282,276 +1447,287 @@
       <c r="H34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="16"/>
+      <c r="B35" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>41</v>
+      </c>
       <c r="D35" s="11" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
     </row>
-    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="15"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="9"/>
-      <c r="E36" s="9"/>
-      <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-    </row>
-    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="15" t="s">
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B36" s="19"/>
+      <c r="C36" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B37" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="D37" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-    </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B38" s="21"/>
-      <c r="C38" s="8" t="s">
+      <c r="C37" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="18"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+    </row>
+    <row r="39" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B39" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="D38" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E38" s="17"/>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="15"/>
-    </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="21"/>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="8" t="s">
         <v>51</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="E39" s="11"/>
       <c r="F39" s="11"/>
       <c r="G39" s="11"/>
       <c r="H39" s="11"/>
-      <c r="I39" s="15"/>
-    </row>
-    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="21"/>
-      <c r="C40" s="15" t="s">
+    </row>
+    <row r="40" customFormat="false" ht="27.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B40" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="D40" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="15"/>
-    </row>
-    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B41" s="21"/>
-      <c r="C41" s="15" t="s">
+      <c r="C40" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D41" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="15"/>
-    </row>
-    <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="21"/>
-      <c r="C42" s="15" t="s">
+      <c r="D40" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="18"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B42" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D42" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="15"/>
-    </row>
-    <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="15"/>
-      <c r="D43" s="9"/>
-      <c r="E43" s="9"/>
-      <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="15"/>
-    </row>
-    <row r="44" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B44" s="22" t="s">
+      <c r="C42" s="18"/>
+      <c r="D42" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B43" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="D44" s="11" t="s">
+      <c r="C43" s="18"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="15"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+    </row>
+    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B45" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="15"/>
-    </row>
-    <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="22"/>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="D45" s="13" t="s">
+      <c r="D45" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B46" s="28"/>
+      <c r="C46" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="15"/>
-    </row>
-    <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="23"/>
-      <c r="G46" s="23"/>
-      <c r="H46" s="23"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
       <c r="I46" s="15"/>
     </row>
-    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C47" s="8" t="s">
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B47" s="28"/>
+      <c r="C47" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="D47" s="11" t="s">
+      <c r="D47" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="15"/>
+    </row>
+    <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B48" s="28"/>
+      <c r="C48" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="15"/>
-    </row>
-    <row r="48" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="10"/>
-      <c r="C48" s="8" t="s">
+      <c r="D48" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="15"/>
+    </row>
+    <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B49" s="28"/>
+      <c r="C49" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D48" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="15"/>
-    </row>
-    <row r="49" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="10"/>
-      <c r="C49" s="8" t="s">
+      <c r="D49" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="15"/>
+    </row>
+    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B50" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="D49" s="24" t="s">
+      <c r="C50" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D50" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E49" s="24"/>
-      <c r="F49" s="24"/>
-      <c r="G49" s="24"/>
-      <c r="H49" s="24"/>
-      <c r="I49" s="15"/>
-    </row>
-    <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D50" s="23"/>
-      <c r="E50" s="23"/>
-      <c r="F50" s="23"/>
-      <c r="G50" s="23"/>
-      <c r="H50" s="23"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
       <c r="I50" s="15"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B51" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C51" s="8"/>
-      <c r="D51" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
+    <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="15"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
       <c r="I51" s="15"/>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C52" s="8"/>
-      <c r="D52" s="9"/>
-      <c r="E52" s="9"/>
-      <c r="F52" s="9"/>
-      <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
+    <row r="52" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B52" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
       <c r="I52" s="15"/>
     </row>
-    <row r="53" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C53" s="27" t="s">
-        <v>66</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
+    <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B53" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
       <c r="I53" s="15"/>
     </row>
-    <row r="54" customFormat="false" ht="68.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="26"/>
-      <c r="C54" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D54" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="E54" s="24"/>
-      <c r="F54" s="24"/>
-      <c r="G54" s="24"/>
-      <c r="H54" s="24"/>
+    <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="29"/>
+      <c r="G54" s="29"/>
+      <c r="H54" s="29"/>
       <c r="I54" s="15"/>
     </row>
-    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B55" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
       <c r="I55" s="15"/>
     </row>
-    <row r="56" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B56" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="C56" s="28" t="s">
-        <v>66</v>
+    <row r="56" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B56" s="10"/>
+      <c r="C56" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E56" s="11"/>
       <c r="F56" s="11"/>
@@ -1559,113 +1735,197 @@
       <c r="H56" s="11"/>
       <c r="I56" s="15"/>
     </row>
-    <row r="57" customFormat="false" ht="55.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B57" s="26"/>
-      <c r="C57" s="29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
+    <row r="57" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B57" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D57" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" s="30"/>
+      <c r="F57" s="30"/>
+      <c r="G57" s="30"/>
+      <c r="H57" s="30"/>
       <c r="I57" s="15"/>
     </row>
-    <row r="58" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="26"/>
-      <c r="C58" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="D58" s="24" t="s">
+    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D58" s="29"/>
+      <c r="E58" s="29"/>
+      <c r="F58" s="29"/>
+      <c r="G58" s="29"/>
+      <c r="H58" s="29"/>
+      <c r="I58" s="15"/>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B59" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="15"/>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B60" s="31"/>
+      <c r="C60" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="D60" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="24"/>
-      <c r="H58" s="24"/>
-      <c r="I58" s="15"/>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="30"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="9"/>
-      <c r="E59" s="9"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="15"/>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="30"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="9"/>
-      <c r="E60" s="9"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
       <c r="I60" s="15"/>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="30"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="9"/>
-      <c r="F61" s="9"/>
-      <c r="G61" s="9"/>
-      <c r="H61" s="9"/>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="30"/>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B61" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="C61" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="15"/>
+    </row>
+    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C62" s="8"/>
       <c r="D62" s="9"/>
       <c r="E62" s="9"/>
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
-    </row>
-    <row r="65" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C67" s="31"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="9"/>
-      <c r="F67" s="9"/>
-      <c r="G67" s="9"/>
-      <c r="H67" s="9"/>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="30"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="9"/>
-      <c r="F68" s="9"/>
-      <c r="G68" s="9"/>
-      <c r="H68" s="9"/>
+      <c r="I62" s="15"/>
+    </row>
+    <row r="63" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B63" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="C63" s="33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D63" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="15"/>
+    </row>
+    <row r="64" customFormat="false" ht="54.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B64" s="32" t="s">
+        <v>83</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D64" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64" s="30"/>
+      <c r="F64" s="30"/>
+      <c r="G64" s="30"/>
+      <c r="H64" s="30"/>
+      <c r="I64" s="15"/>
+    </row>
+    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I65" s="15"/>
+    </row>
+    <row r="66" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B66" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="C66" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D66" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="15"/>
+    </row>
+    <row r="67" customFormat="false" ht="55.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B67" s="32"/>
+      <c r="C67" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
+      <c r="I67" s="15"/>
+    </row>
+    <row r="68" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B68" s="32" t="s">
+        <v>87</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D68" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="E68" s="30"/>
+      <c r="F68" s="30"/>
+      <c r="G68" s="30"/>
+      <c r="H68" s="30"/>
+      <c r="I68" s="15"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="30"/>
+      <c r="B69" s="35"/>
+      <c r="C69" s="8"/>
       <c r="D69" s="9"/>
       <c r="E69" s="9"/>
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
       <c r="H69" s="9"/>
-    </row>
-    <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I69" s="15"/>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="35"/>
+      <c r="C70" s="8"/>
       <c r="D70" s="9"/>
       <c r="E70" s="9"/>
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
       <c r="H70" s="9"/>
+      <c r="I70" s="15"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="30"/>
+      <c r="B71" s="35"/>
+      <c r="C71" s="8"/>
       <c r="D71" s="9"/>
       <c r="E71" s="9"/>
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
       <c r="H71" s="9"/>
     </row>
-    <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="35"/>
       <c r="C72" s="8"/>
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
@@ -1673,45 +1933,9 @@
       <c r="G72" s="9"/>
       <c r="H72" s="9"/>
     </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="30"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="9"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="9"/>
-      <c r="G73" s="9"/>
-      <c r="H73" s="9"/>
-    </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="30"/>
-      <c r="C74" s="8"/>
-      <c r="D74" s="9"/>
-      <c r="E74" s="9"/>
-      <c r="F74" s="9"/>
-      <c r="G74" s="9"/>
-      <c r="H74" s="9"/>
-    </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="32"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="9"/>
-      <c r="E75" s="9"/>
-      <c r="F75" s="9"/>
-      <c r="G75" s="9"/>
-      <c r="H75" s="9"/>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="30"/>
-      <c r="C76" s="8"/>
-      <c r="D76" s="9"/>
-      <c r="E76" s="9"/>
-      <c r="F76" s="9"/>
-      <c r="G76" s="9"/>
-      <c r="H76" s="9"/>
-    </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="30"/>
-      <c r="C77" s="8"/>
+    <row r="75" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C77" s="36"/>
       <c r="D77" s="9"/>
       <c r="E77" s="9"/>
       <c r="F77" s="9"/>
@@ -1719,8 +1943,7 @@
       <c r="H77" s="9"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="30"/>
-      <c r="C78" s="8"/>
+      <c r="B78" s="35"/>
       <c r="D78" s="9"/>
       <c r="E78" s="9"/>
       <c r="F78" s="9"/>
@@ -1728,17 +1951,14 @@
       <c r="H78" s="9"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="30"/>
-      <c r="C79" s="8"/>
+      <c r="B79" s="35"/>
       <c r="D79" s="9"/>
       <c r="E79" s="9"/>
       <c r="F79" s="9"/>
       <c r="G79" s="9"/>
       <c r="H79" s="9"/>
     </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="32"/>
-      <c r="C80" s="8"/>
+    <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
       <c r="F80" s="9"/>
@@ -1746,16 +1966,14 @@
       <c r="H80" s="9"/>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="30"/>
-      <c r="C81" s="8"/>
+      <c r="B81" s="35"/>
       <c r="D81" s="9"/>
       <c r="E81" s="9"/>
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
       <c r="H81" s="9"/>
     </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="30"/>
+    <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C82" s="8"/>
       <c r="D82" s="9"/>
       <c r="E82" s="9"/>
@@ -1764,8 +1982,8 @@
       <c r="H82" s="9"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="30"/>
-      <c r="C83" s="31"/>
+      <c r="B83" s="35"/>
+      <c r="C83" s="8"/>
       <c r="D83" s="9"/>
       <c r="E83" s="9"/>
       <c r="F83" s="9"/>
@@ -1773,8 +1991,8 @@
       <c r="H83" s="9"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="30"/>
-      <c r="C84" s="31"/>
+      <c r="B84" s="35"/>
+      <c r="C84" s="8"/>
       <c r="D84" s="9"/>
       <c r="E84" s="9"/>
       <c r="F84" s="9"/>
@@ -1782,8 +2000,8 @@
       <c r="H84" s="9"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="30"/>
-      <c r="C85" s="31"/>
+      <c r="B85" s="37"/>
+      <c r="C85" s="8"/>
       <c r="D85" s="9"/>
       <c r="E85" s="9"/>
       <c r="F85" s="9"/>
@@ -1791,8 +2009,8 @@
       <c r="H85" s="9"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="30"/>
-      <c r="C86" s="31"/>
+      <c r="B86" s="35"/>
+      <c r="C86" s="8"/>
       <c r="D86" s="9"/>
       <c r="E86" s="9"/>
       <c r="F86" s="9"/>
@@ -1800,8 +2018,8 @@
       <c r="H86" s="9"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="30"/>
-      <c r="C87" s="31"/>
+      <c r="B87" s="35"/>
+      <c r="C87" s="8"/>
       <c r="D87" s="9"/>
       <c r="E87" s="9"/>
       <c r="F87" s="9"/>
@@ -1809,8 +2027,8 @@
       <c r="H87" s="9"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="30"/>
-      <c r="C88" s="31"/>
+      <c r="B88" s="35"/>
+      <c r="C88" s="8"/>
       <c r="D88" s="9"/>
       <c r="E88" s="9"/>
       <c r="F88" s="9"/>
@@ -1818,7 +2036,8 @@
       <c r="H88" s="9"/>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="30"/>
+      <c r="B89" s="35"/>
+      <c r="C89" s="8"/>
       <c r="D89" s="9"/>
       <c r="E89" s="9"/>
       <c r="F89" s="9"/>
@@ -1826,7 +2045,8 @@
       <c r="H89" s="9"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="30"/>
+      <c r="B90" s="37"/>
+      <c r="C90" s="8"/>
       <c r="D90" s="9"/>
       <c r="E90" s="9"/>
       <c r="F90" s="9"/>
@@ -1834,7 +2054,8 @@
       <c r="H90" s="9"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="30"/>
+      <c r="B91" s="35"/>
+      <c r="C91" s="8"/>
       <c r="D91" s="9"/>
       <c r="E91" s="9"/>
       <c r="F91" s="9"/>
@@ -1842,7 +2063,8 @@
       <c r="H91" s="9"/>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="33"/>
+      <c r="B92" s="35"/>
+      <c r="C92" s="8"/>
       <c r="D92" s="9"/>
       <c r="E92" s="9"/>
       <c r="F92" s="9"/>
@@ -1850,7 +2072,8 @@
       <c r="H92" s="9"/>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="33"/>
+      <c r="B93" s="35"/>
+      <c r="C93" s="36"/>
       <c r="D93" s="9"/>
       <c r="E93" s="9"/>
       <c r="F93" s="9"/>
@@ -1858,7 +2081,8 @@
       <c r="H93" s="9"/>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="33"/>
+      <c r="B94" s="35"/>
+      <c r="C94" s="36"/>
       <c r="D94" s="9"/>
       <c r="E94" s="9"/>
       <c r="F94" s="9"/>
@@ -1866,7 +2090,8 @@
       <c r="H94" s="9"/>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="33"/>
+      <c r="B95" s="35"/>
+      <c r="C95" s="36"/>
       <c r="D95" s="9"/>
       <c r="E95" s="9"/>
       <c r="F95" s="9"/>
@@ -1874,7 +2099,8 @@
       <c r="H95" s="9"/>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="33"/>
+      <c r="B96" s="35"/>
+      <c r="C96" s="36"/>
       <c r="D96" s="9"/>
       <c r="E96" s="9"/>
       <c r="F96" s="9"/>
@@ -1882,7 +2108,8 @@
       <c r="H96" s="9"/>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="33"/>
+      <c r="B97" s="35"/>
+      <c r="C97" s="36"/>
       <c r="D97" s="9"/>
       <c r="E97" s="9"/>
       <c r="F97" s="9"/>
@@ -1890,7 +2117,8 @@
       <c r="H97" s="9"/>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="33"/>
+      <c r="B98" s="35"/>
+      <c r="C98" s="36"/>
       <c r="D98" s="9"/>
       <c r="E98" s="9"/>
       <c r="F98" s="9"/>
@@ -1898,7 +2126,7 @@
       <c r="H98" s="9"/>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="33"/>
+      <c r="B99" s="35"/>
       <c r="D99" s="9"/>
       <c r="E99" s="9"/>
       <c r="F99" s="9"/>
@@ -1906,7 +2134,7 @@
       <c r="H99" s="9"/>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="33"/>
+      <c r="B100" s="35"/>
       <c r="D100" s="9"/>
       <c r="E100" s="9"/>
       <c r="F100" s="9"/>
@@ -1914,7 +2142,7 @@
       <c r="H100" s="9"/>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="33"/>
+      <c r="B101" s="35"/>
       <c r="D101" s="9"/>
       <c r="E101" s="9"/>
       <c r="F101" s="9"/>
@@ -1922,77 +2150,87 @@
       <c r="H101" s="9"/>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="33"/>
+      <c r="B102" s="38"/>
       <c r="D102" s="9"/>
       <c r="E102" s="9"/>
       <c r="F102" s="9"/>
       <c r="G102" s="9"/>
       <c r="H102" s="9"/>
     </row>
-    <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B103" s="38"/>
       <c r="D103" s="9"/>
       <c r="E103" s="9"/>
       <c r="F103" s="9"/>
       <c r="G103" s="9"/>
       <c r="H103" s="9"/>
     </row>
-    <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B104" s="38"/>
       <c r="D104" s="9"/>
       <c r="E104" s="9"/>
       <c r="F104" s="9"/>
       <c r="G104" s="9"/>
       <c r="H104" s="9"/>
     </row>
-    <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B105" s="38"/>
       <c r="D105" s="9"/>
       <c r="E105" s="9"/>
       <c r="F105" s="9"/>
       <c r="G105" s="9"/>
       <c r="H105" s="9"/>
     </row>
-    <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B106" s="38"/>
       <c r="D106" s="9"/>
       <c r="E106" s="9"/>
       <c r="F106" s="9"/>
       <c r="G106" s="9"/>
       <c r="H106" s="9"/>
     </row>
-    <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B107" s="38"/>
       <c r="D107" s="9"/>
       <c r="E107" s="9"/>
       <c r="F107" s="9"/>
       <c r="G107" s="9"/>
       <c r="H107" s="9"/>
     </row>
-    <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B108" s="38"/>
       <c r="D108" s="9"/>
       <c r="E108" s="9"/>
       <c r="F108" s="9"/>
       <c r="G108" s="9"/>
       <c r="H108" s="9"/>
     </row>
-    <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B109" s="38"/>
       <c r="D109" s="9"/>
       <c r="E109" s="9"/>
       <c r="F109" s="9"/>
       <c r="G109" s="9"/>
       <c r="H109" s="9"/>
     </row>
-    <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B110" s="38"/>
       <c r="D110" s="9"/>
       <c r="E110" s="9"/>
       <c r="F110" s="9"/>
       <c r="G110" s="9"/>
       <c r="H110" s="9"/>
     </row>
-    <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B111" s="38"/>
       <c r="D111" s="9"/>
       <c r="E111" s="9"/>
       <c r="F111" s="9"/>
       <c r="G111" s="9"/>
       <c r="H111" s="9"/>
     </row>
-    <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B112" s="38"/>
       <c r="D112" s="9"/>
       <c r="E112" s="9"/>
       <c r="F112" s="9"/>
@@ -2447,8 +2685,78 @@
       <c r="G176" s="9"/>
       <c r="H176" s="9"/>
     </row>
+    <row r="177" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D177" s="9"/>
+      <c r="E177" s="9"/>
+      <c r="F177" s="9"/>
+      <c r="G177" s="9"/>
+      <c r="H177" s="9"/>
+    </row>
+    <row r="178" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D178" s="9"/>
+      <c r="E178" s="9"/>
+      <c r="F178" s="9"/>
+      <c r="G178" s="9"/>
+      <c r="H178" s="9"/>
+    </row>
+    <row r="179" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D179" s="9"/>
+      <c r="E179" s="9"/>
+      <c r="F179" s="9"/>
+      <c r="G179" s="9"/>
+      <c r="H179" s="9"/>
+    </row>
+    <row r="180" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D180" s="9"/>
+      <c r="E180" s="9"/>
+      <c r="F180" s="9"/>
+      <c r="G180" s="9"/>
+      <c r="H180" s="9"/>
+    </row>
+    <row r="181" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D181" s="9"/>
+      <c r="E181" s="9"/>
+      <c r="F181" s="9"/>
+      <c r="G181" s="9"/>
+      <c r="H181" s="9"/>
+    </row>
+    <row r="182" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D182" s="9"/>
+      <c r="E182" s="9"/>
+      <c r="F182" s="9"/>
+      <c r="G182" s="9"/>
+      <c r="H182" s="9"/>
+    </row>
+    <row r="183" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D183" s="9"/>
+      <c r="E183" s="9"/>
+      <c r="F183" s="9"/>
+      <c r="G183" s="9"/>
+      <c r="H183" s="9"/>
+    </row>
+    <row r="184" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D184" s="9"/>
+      <c r="E184" s="9"/>
+      <c r="F184" s="9"/>
+      <c r="G184" s="9"/>
+      <c r="H184" s="9"/>
+    </row>
+    <row r="185" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D185" s="9"/>
+      <c r="E185" s="9"/>
+      <c r="F185" s="9"/>
+      <c r="G185" s="9"/>
+      <c r="H185" s="9"/>
+    </row>
+    <row r="186" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D186" s="9"/>
+      <c r="E186" s="9"/>
+      <c r="F186" s="9"/>
+      <c r="G186" s="9"/>
+      <c r="H186" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="181">
+  <mergeCells count="189">
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:M2"/>
     <mergeCell ref="B3:H3"/>
@@ -2456,14 +2764,13 @@
     <mergeCell ref="D4:H4"/>
     <mergeCell ref="K4:M4"/>
     <mergeCell ref="D5:H5"/>
-    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="B6:B16"/>
     <mergeCell ref="D6:H6"/>
     <mergeCell ref="D7:H7"/>
     <mergeCell ref="D8:H8"/>
     <mergeCell ref="D9:H9"/>
     <mergeCell ref="D10:H10"/>
     <mergeCell ref="D11:H11"/>
-    <mergeCell ref="B12:B17"/>
     <mergeCell ref="D12:H12"/>
     <mergeCell ref="D13:H13"/>
     <mergeCell ref="D14:H14"/>
@@ -2483,53 +2790,52 @@
     <mergeCell ref="D27:H27"/>
     <mergeCell ref="D28:H28"/>
     <mergeCell ref="D29:H29"/>
+    <mergeCell ref="B30:B32"/>
     <mergeCell ref="D30:H30"/>
     <mergeCell ref="D31:H31"/>
     <mergeCell ref="D32:H32"/>
     <mergeCell ref="D33:H33"/>
     <mergeCell ref="D34:H34"/>
+    <mergeCell ref="B35:B36"/>
     <mergeCell ref="D35:H35"/>
     <mergeCell ref="D36:H36"/>
-    <mergeCell ref="B37:B42"/>
     <mergeCell ref="D37:H37"/>
     <mergeCell ref="D38:H38"/>
     <mergeCell ref="D39:H39"/>
     <mergeCell ref="D40:H40"/>
     <mergeCell ref="D41:H41"/>
-    <mergeCell ref="D42:H42"/>
-    <mergeCell ref="D43:H43"/>
-    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="D42:H43"/>
     <mergeCell ref="D44:H44"/>
+    <mergeCell ref="B45:B49"/>
     <mergeCell ref="D45:H45"/>
     <mergeCell ref="D46:H46"/>
-    <mergeCell ref="B47:B49"/>
     <mergeCell ref="D47:H47"/>
     <mergeCell ref="D48:H48"/>
     <mergeCell ref="D49:H49"/>
     <mergeCell ref="D50:H50"/>
     <mergeCell ref="D51:H51"/>
     <mergeCell ref="D52:H52"/>
-    <mergeCell ref="B53:B54"/>
     <mergeCell ref="D53:H53"/>
     <mergeCell ref="D54:H54"/>
-    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="D55:H55"/>
     <mergeCell ref="D56:H56"/>
     <mergeCell ref="D57:H57"/>
     <mergeCell ref="D58:H58"/>
+    <mergeCell ref="B59:B60"/>
     <mergeCell ref="D59:H59"/>
     <mergeCell ref="D60:H60"/>
     <mergeCell ref="D61:H61"/>
     <mergeCell ref="D62:H62"/>
+    <mergeCell ref="D63:H63"/>
+    <mergeCell ref="D64:H64"/>
+    <mergeCell ref="D66:H66"/>
     <mergeCell ref="D67:H67"/>
     <mergeCell ref="D68:H68"/>
     <mergeCell ref="D69:H69"/>
     <mergeCell ref="D70:H70"/>
     <mergeCell ref="D71:H71"/>
     <mergeCell ref="D72:H72"/>
-    <mergeCell ref="D73:H73"/>
-    <mergeCell ref="D74:H74"/>
-    <mergeCell ref="D75:H75"/>
-    <mergeCell ref="D76:H76"/>
     <mergeCell ref="D77:H77"/>
     <mergeCell ref="D78:H78"/>
     <mergeCell ref="D79:H79"/>
@@ -2630,6 +2936,16 @@
     <mergeCell ref="D174:H174"/>
     <mergeCell ref="D175:H175"/>
     <mergeCell ref="D176:H176"/>
+    <mergeCell ref="D177:H177"/>
+    <mergeCell ref="D178:H178"/>
+    <mergeCell ref="D179:H179"/>
+    <mergeCell ref="D180:H180"/>
+    <mergeCell ref="D181:H181"/>
+    <mergeCell ref="D182:H182"/>
+    <mergeCell ref="D183:H183"/>
+    <mergeCell ref="D184:H184"/>
+    <mergeCell ref="D185:H185"/>
+    <mergeCell ref="D186:H186"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
updated KNIME_nodes_MD4DSP_mapping.xlsx with join new transformation
</commit_message>
<xml_diff>
--- a/KNIME_nodes_MD4DSP_mapping.xlsx
+++ b/KNIME_nodes_MD4DSP_mapping.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="93">
   <si>
     <t xml:space="preserve">No contemplado en nuestra librería</t>
   </si>
@@ -348,98 +348,708 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">rowFilter type: include rows by attribute value | </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">matching criteria: use pattern matching</t>
+      <t xml:space="preserve">rowFilter type:</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> include rows by attribute value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> | matching criteria: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">use pattern matching</t>
     </r>
   </si>
   <si>
     <t xml:space="preserve">rowFilterPrimitive</t>
   </si>
   <si>
-    <t xml:space="preserve">rowFilter type: include rows by attribute value | matching criteria: use range checking</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">rowFilter type:</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> include rows by attribute value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> | matching criteria:</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> use range checking</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">rowFilterRange</t>
   </si>
   <si>
-    <t xml:space="preserve">rowFilter type: include rows by attribute value | matching criteria: only missing values match</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">rowFilter type: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">include rows by attribute value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> | matching criteria: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">only missing values match</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">rowFilterMissing</t>
   </si>
   <si>
-    <t xml:space="preserve">rowFilter type: exclude rows by attribute value | matching criteria: use pattern matching</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilter type: exclude rows by attribute value | matching criteria: use range checking</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilter type: exclude rows by attribute value | matching criteria: only missing values match</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilter type: include rows by number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilter type: exclude rows by number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rowFilter type: include rows by rowID</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">rowFilter type:</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> exclude rows by attribute value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> | matching criteria:</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> use pattern matching</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">rowFilter type: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">exclude rows by attribute value </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">| matching criteria: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">use range checking</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">rowFilter type: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">exclude rows by attribute value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> | matching criteria: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">only missing values match</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">rowFilter type: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">include rows by number</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">rowFilter type: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">exclude rows by number</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">rowFilter type: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">include rows by rowID</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">6/10  configuraciones mapeadas – 60%</t>
   </si>
   <si>
-    <t xml:space="preserve">rowFilter type: exclude rows by rowID</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">rowFilter type: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">exclude rows by rowID</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Column Filter</t>
   </si>
   <si>
-    <t xml:space="preserve">included_columns --&gt; out_columns | Column filter option: Manual</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">included_columns --&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">out_columns</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> | Column filter option: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Manual</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">columnFilter</t>
   </si>
   <si>
-    <t xml:space="preserve">included_columns --&gt; out_columns | Column filter option: Wildcard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">included_columns --&gt; out_columns | Column filter option: Regex</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">included_columns --&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> out_columns </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">| Column filter option: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Wildcard</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">included_columns --&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> out_columns </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">| Column filter option: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Regex</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">¼ configuraciones mapeadas – 25%</t>
   </si>
   <si>
-    <t xml:space="preserve">included_columns --&gt; out_columns | Column filter option: Type</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">included_columns --&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> out_columns</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> | Column filter option: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Type</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">String to Number</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">included_columns --&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">out_columns </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">| Column filter option: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Manual</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">categoricalToContinuous</t>
   </si>
   <si>
     <t xml:space="preserve">1/3 configuraciones mapeadas – 33%</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">included_columns --&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">out_columns </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">| Column filter option: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Regex</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Numeric Outliers</t>
   </si>
   <si>
-    <t xml:space="preserve">Sólo mappeado para la configuración - convertir todos los Outliers al valor permitido más cercano utilizando el cálculo de cuartil R_4 y el multiplicador de rango intercuartílico: 1.5</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Sólo mappeado para la configuración - convertir todos los </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Outliers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> al valor permitido más cercano utilizando el cálculo de cuartil R_4 y el multiplicador de rango intercuartílico: 1.5</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">configuraciones mapeadas – SIN DETERMINAR</t>
   </si>
   <si>
-    <t xml:space="preserve">Resto de configuraciones relativas a los parámetros: Interquartile range multiplier (k), quartile calculation, Oulier treatment: apply to., treatment option, replacement strategy</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Resto de configuraciones relativas a los parámetros: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Interquartile range multiplier (k), quartile calculation, Oulier treatment: apply to., treatment option, replacement strategy</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Numeric Binner</t>
@@ -462,77 +1072,299 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Binning method: fixed number of bins | </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Bin_naming: numbered</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Binning method: Sample quantiles </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">| Bin_naming: numbered</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Binning method: fixed number of bins | </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Bin_naming: borders</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Binning method: Sample quantiles | Bin_naming: borders</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Binning method: fixed number of bins | Bin_naming: midpoints</t>
+      <t xml:space="preserve">Binning method: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">fixed number of bins</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> | Bin_naming: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">numbered</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Binning method: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Sample quantiles</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> | Bin_naming: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">numbered</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Binning method: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">fixed number of bins</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> | Bin_naming: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">borders</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Binning method:</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Sample quantiles </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">| Bin_naming: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">borders</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Binning method: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">fixed number of bins </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">| Bin_naming: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">midpoints</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">1/6 configuraciones mapeadas – 16%</t>
   </si>
   <si>
-    <t xml:space="preserve">Binning method: Sample quantiles | Bin_naming: midpoints</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Binning method: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Sample quantiles </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">| Bin_naming: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">midpoints</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Math Formula</t>
   </si>
   <si>
-    <t xml:space="preserve">Limitación de mapping - Sólo hecho para dos operandos (columnas o valores fijos) de operaciones SUMA, RESTA, MULTIPLICACIÓN y DIVISIÓN. El mapping del resto de operaciones mátemáticas queda para ser extendidas en el futuro, así como un número diferente de operandos. Mapeo actual: caso base con 2 operandos y 1 operador.</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Limitación de Math Formula - </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Sólo hecho para dos operandos (columnas o valores fijos) de operaciones SUMA, RESTA, MULTIPLICACIÓN y DIVISIÓN.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> El mapping del resto de operaciones mátemáticas queda para ser extendidas en el futuro, así como un número diferente de operandos. Mapeo actual: caso base con 2 operandos y 1 operador.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">mathOpFieldField / mathOpFieldFixValue</t>
@@ -565,7 +1397,27 @@
     <t xml:space="preserve">String Replacer</t>
   </si>
   <si>
-    <t xml:space="preserve">Patern – Replacement text | Replacement type: Literal</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Patern – Replacement text | Replacement type: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Literal</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Patern – Replacement text | Replacement type: Wildcard</t>
@@ -580,19 +1432,95 @@
     <t xml:space="preserve">String Manipulation - String Manipulation (Multi Column)</t>
   </si>
   <si>
-    <t xml:space="preserve">Expresión con function: replace, replaceChars o substr. Limitación para aplicarlo sobre una sóla columna de entrada</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Expresión con function: </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">replace, replaceChars o substr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. Limitación para aplicarlo sobre una sóla columna de entrada</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Expresión de concatenación de strings con múltiples operandos </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">(pueden ser columnas o valores fijos)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">join</t>
   </si>
   <si>
     <t xml:space="preserve">3/53 configuraciones mapeadas – 5.6%</t>
   </si>
   <si>
-    <t xml:space="preserve">Functions: capitalize, removeChars, compare, count, countChars, indexOf, indexOfChars, join, joinStep, lastIndexOfChar, length, lowerCase, upperCase, md5Checksum, padLeft, padRight, regexMatcher, removeChars, removeDiacritic, removeDuplicates, regexReplace, removeUmlauts, reverse, string, strip, stripEnd, stripStart, toBoolean, toDouble, toInt, toLong, toNull, toEmpty, urlEncode, urlDecode. Tampoco es posible mappear funciones anidadas. Un ejemplo de función no mappeada es la función join($Name$, " - ", $City$)</t>
+    <t xml:space="preserve">Functions: capitalize, removeChars, compare, count, countChars, indexOf, indexOfChars, joinStep, lastIndexOfChar, length, lowerCase, upperCase, md5Checksum, padLeft, padRight, regexMatcher, removeChars, removeDiacritic, removeDuplicates, regexReplace, removeUmlauts, reverse, string, strip, stripEnd, stripStart, toBoolean, toDouble, toInt, toLong, toNull, toEmpty, urlEncode, urlDecode. Tampoco es posible mappear funciones anidadas.</t>
   </si>
   <si>
     <t xml:space="preserve">Column Expressions</t>
   </si>
   <si>
-    <t xml:space="preserve">Expresión matemática únicamente con dos operandos (columnas o valores fijos) de operaciones SUMA, RESTA, MULTIPLICACIÓN y DIVISIÓN. El mapping del resto de operaciones mátemáticas queda para ser extendidas en el futuro, así como un número diferente de operandos, así como ocurre en el mapeo de dichas operaciones para el nodo MathFormula</t>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Expresión matemática únicamente con dos operandos (columnas o valores fijos) de operaciones SUMA, RESTA, MULTIPLICACIÓN y DIVISIÓN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">. El mapping del resto de operaciones mátemáticas queda para ser extendidas en el futuro, así como un número diferente de operandos, así como ocurre en el mapeo de dichas operaciones para el nodo MathFormula</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">7/185 configuraciones mapeadas – 3.78%</t>
@@ -609,7 +1537,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -667,18 +1595,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="JetBrains Mono"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -690,6 +1606,14 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
@@ -764,7 +1688,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="34">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -821,19 +1745,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -841,27 +1753,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -869,7 +1773,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -877,7 +1781,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -885,11 +1789,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -897,19 +1801,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -917,7 +1821,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -998,10 +1902,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:M186"/>
+  <dimension ref="B1:M187"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D68" activeCellId="0" sqref="D68"/>
+      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1218,7 +2122,7 @@
       <c r="H16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="10" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="12" t="s">
@@ -1243,20 +2147,20 @@
       <c r="B19" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="10"/>
-      <c r="C20" s="17" t="s">
+      <c r="C20" s="14" t="s">
         <v>28</v>
       </c>
       <c r="D20" s="11" t="s">
@@ -1269,7 +2173,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="10"/>
-      <c r="C21" s="17" t="s">
+      <c r="C21" s="14" t="s">
         <v>30</v>
       </c>
       <c r="D21" s="11" t="s">
@@ -1282,20 +2186,20 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="10"/>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="10"/>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="14" t="s">
         <v>33</v>
       </c>
       <c r="D23" s="11" t="s">
@@ -1308,7 +2212,7 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="10"/>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="14" t="s">
         <v>34</v>
       </c>
       <c r="D24" s="11" t="s">
@@ -1321,7 +2225,7 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B25" s="10"/>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D25" s="13" t="s">
@@ -1334,7 +2238,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B26" s="10"/>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="15" t="s">
         <v>36</v>
       </c>
       <c r="D26" s="13" t="s">
@@ -1347,7 +2251,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B27" s="10"/>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D27" s="13" t="s">
@@ -1359,10 +2263,10 @@
       <c r="H27" s="13"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="15" t="s">
         <v>39</v>
       </c>
       <c r="D28" s="13" t="s">
@@ -1382,7 +2286,7 @@
       <c r="H29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="16" t="s">
         <v>40</v>
       </c>
       <c r="C30" s="8" t="s">
@@ -1397,8 +2301,8 @@
       <c r="H30" s="11"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="19"/>
-      <c r="C31" s="20" t="s">
+      <c r="B31" s="16"/>
+      <c r="C31" s="12" t="s">
         <v>43</v>
       </c>
       <c r="D31" s="13" t="s">
@@ -1410,8 +2314,8 @@
       <c r="H31" s="13"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B32" s="19"/>
-      <c r="C32" s="20" t="s">
+      <c r="B32" s="16"/>
+      <c r="C32" s="12" t="s">
         <v>44</v>
       </c>
       <c r="D32" s="13" t="s">
@@ -1423,10 +2327,10 @@
       <c r="H32" s="13"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="21" t="s">
+      <c r="B33" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="12" t="s">
         <v>46</v>
       </c>
       <c r="D33" s="13" t="s">
@@ -1438,7 +2342,7 @@
       <c r="H33" s="13"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="22"/>
+      <c r="B34" s="18"/>
       <c r="C34" s="8"/>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
@@ -1447,14 +2351,14 @@
       <c r="H34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="18" t="s">
-        <v>41</v>
+      <c r="C35" s="15" t="s">
+        <v>48</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
@@ -1462,8 +2366,8 @@
       <c r="H35" s="11"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B36" s="19"/>
-      <c r="C36" s="23" t="s">
+      <c r="B36" s="16"/>
+      <c r="C36" s="15" t="s">
         <v>43</v>
       </c>
       <c r="D36" s="13" t="s">
@@ -1475,11 +2379,11 @@
       <c r="H36" s="13"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" s="23" t="s">
-        <v>44</v>
+      <c r="B37" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>51</v>
       </c>
       <c r="D37" s="13" t="s">
         <v>15</v>
@@ -1490,7 +2394,7 @@
       <c r="H37" s="13"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="18"/>
+      <c r="B38" s="15"/>
       <c r="C38" s="8"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
@@ -1499,11 +2403,11 @@
       <c r="H38" s="9"/>
     </row>
     <row r="39" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B39" s="19" t="s">
-        <v>50</v>
+      <c r="B39" s="20" t="s">
+        <v>52</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>20</v>
@@ -1514,11 +2418,11 @@
       <c r="H39" s="11"/>
     </row>
     <row r="40" customFormat="false" ht="27.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="25" t="s">
-        <v>52</v>
+      <c r="B40" s="21" t="s">
+        <v>54</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D40" s="13" t="s">
         <v>15</v>
@@ -1529,7 +2433,7 @@
       <c r="H40" s="13"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="18"/>
+      <c r="B41" s="15"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
       <c r="F41" s="9"/>
@@ -1537,12 +2441,12 @@
       <c r="H41" s="9"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B42" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="C42" s="18"/>
+      <c r="B42" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="15"/>
       <c r="D42" s="11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E42" s="11"/>
       <c r="F42" s="11"/>
@@ -1550,10 +2454,10 @@
       <c r="H42" s="11"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B43" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="C43" s="18"/>
+      <c r="B43" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="15"/>
       <c r="D43" s="11"/>
       <c r="E43" s="11"/>
       <c r="F43" s="11"/>
@@ -1561,7 +2465,7 @@
       <c r="H43" s="11"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="15"/>
+      <c r="B44" s="14"/>
       <c r="C44" s="8"/>
       <c r="D44" s="9"/>
       <c r="E44" s="9"/>
@@ -1570,14 +2474,14 @@
       <c r="H44" s="9"/>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B45" s="28" t="s">
+      <c r="B45" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" s="11" t="s">
         <v>57</v>
-      </c>
-      <c r="C45" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>55</v>
       </c>
       <c r="E45" s="11"/>
       <c r="F45" s="11"/>
@@ -1585,9 +2489,9 @@
       <c r="H45" s="11"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B46" s="28"/>
+      <c r="B46" s="16"/>
       <c r="C46" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D46" s="13" t="s">
         <v>15</v>
@@ -1596,12 +2500,12 @@
       <c r="F46" s="13"/>
       <c r="G46" s="13"/>
       <c r="H46" s="13"/>
-      <c r="I46" s="15"/>
+      <c r="I46" s="14"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B47" s="28"/>
-      <c r="C47" s="17" t="s">
-        <v>60</v>
+      <c r="B47" s="16"/>
+      <c r="C47" s="14" t="s">
+        <v>62</v>
       </c>
       <c r="D47" s="13" t="s">
         <v>15</v>
@@ -1610,12 +2514,12 @@
       <c r="F47" s="13"/>
       <c r="G47" s="13"/>
       <c r="H47" s="13"/>
-      <c r="I47" s="15"/>
+      <c r="I47" s="14"/>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B48" s="28"/>
-      <c r="C48" s="17" t="s">
-        <v>61</v>
+      <c r="B48" s="16"/>
+      <c r="C48" s="14" t="s">
+        <v>63</v>
       </c>
       <c r="D48" s="13" t="s">
         <v>15</v>
@@ -1624,12 +2528,12 @@
       <c r="F48" s="13"/>
       <c r="G48" s="13"/>
       <c r="H48" s="13"/>
-      <c r="I48" s="15"/>
+      <c r="I48" s="14"/>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B49" s="28"/>
-      <c r="C49" s="17" t="s">
-        <v>62</v>
+      <c r="B49" s="16"/>
+      <c r="C49" s="14" t="s">
+        <v>64</v>
       </c>
       <c r="D49" s="13" t="s">
         <v>15</v>
@@ -1638,14 +2542,14 @@
       <c r="F49" s="13"/>
       <c r="G49" s="13"/>
       <c r="H49" s="13"/>
-      <c r="I49" s="15"/>
+      <c r="I49" s="14"/>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B50" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>64</v>
+      <c r="B50" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="D50" s="13" t="s">
         <v>15</v>
@@ -1654,39 +2558,39 @@
       <c r="F50" s="13"/>
       <c r="G50" s="13"/>
       <c r="H50" s="13"/>
-      <c r="I50" s="15"/>
+      <c r="I50" s="14"/>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="15"/>
+      <c r="B51" s="14"/>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
-      <c r="I51" s="15"/>
+      <c r="I51" s="14"/>
     </row>
     <row r="52" customFormat="false" ht="72" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B52" s="28" t="s">
-        <v>65</v>
+      <c r="B52" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E52" s="11"/>
       <c r="F52" s="11"/>
       <c r="G52" s="11"/>
       <c r="H52" s="11"/>
-      <c r="I52" s="15"/>
+      <c r="I52" s="14"/>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B53" s="28" t="s">
-        <v>68</v>
+      <c r="B53" s="16" t="s">
+        <v>70</v>
       </c>
       <c r="C53" s="8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D53" s="13" t="s">
         <v>15</v>
@@ -1695,90 +2599,90 @@
       <c r="F53" s="13"/>
       <c r="G53" s="13"/>
       <c r="H53" s="13"/>
-      <c r="I53" s="15"/>
+      <c r="I53" s="14"/>
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D54" s="29"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="29"/>
-      <c r="H54" s="29"/>
-      <c r="I54" s="15"/>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="24"/>
+      <c r="H54" s="24"/>
+      <c r="I54" s="14"/>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B55" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="C55" s="25" t="s">
+        <v>73</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E55" s="11"/>
       <c r="F55" s="11"/>
       <c r="G55" s="11"/>
       <c r="H55" s="11"/>
-      <c r="I55" s="15"/>
+      <c r="I55" s="14"/>
     </row>
     <row r="56" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B56" s="10"/>
-      <c r="C56" s="8" t="s">
-        <v>73</v>
+      <c r="C56" s="25" t="s">
+        <v>75</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E56" s="11"/>
       <c r="F56" s="11"/>
       <c r="G56" s="11"/>
       <c r="H56" s="11"/>
-      <c r="I56" s="15"/>
+      <c r="I56" s="14"/>
     </row>
     <row r="57" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D57" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" s="26"/>
+      <c r="F57" s="26"/>
+      <c r="G57" s="26"/>
+      <c r="H57" s="26"/>
+      <c r="I57" s="14"/>
+    </row>
+    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D58" s="24"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="14"/>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B59" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D59" s="11" t="s">
         <v>74</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D57" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="E57" s="30"/>
-      <c r="F57" s="30"/>
-      <c r="G57" s="30"/>
-      <c r="H57" s="30"/>
-      <c r="I57" s="15"/>
-    </row>
-    <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D58" s="29"/>
-      <c r="E58" s="29"/>
-      <c r="F58" s="29"/>
-      <c r="G58" s="29"/>
-      <c r="H58" s="29"/>
-      <c r="I58" s="15"/>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B59" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="C59" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D59" s="11" t="s">
-        <v>72</v>
       </c>
       <c r="E59" s="11"/>
       <c r="F59" s="11"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
-      <c r="I59" s="15"/>
+      <c r="I59" s="14"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B60" s="31"/>
-      <c r="C60" s="23" t="s">
-        <v>78</v>
+      <c r="B60" s="10"/>
+      <c r="C60" s="15" t="s">
+        <v>80</v>
       </c>
       <c r="D60" s="13" t="s">
         <v>15</v>
@@ -1787,14 +2691,14 @@
       <c r="F60" s="13"/>
       <c r="G60" s="13"/>
       <c r="H60" s="13"/>
-      <c r="I60" s="15"/>
+      <c r="I60" s="14"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B61" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="C61" s="23" t="s">
-        <v>80</v>
+      <c r="B61" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="D61" s="13" t="s">
         <v>15</v>
@@ -1803,7 +2707,7 @@
       <c r="F61" s="13"/>
       <c r="G61" s="13"/>
       <c r="H61" s="13"/>
-      <c r="I61" s="15"/>
+      <c r="I61" s="14"/>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C62" s="8"/>
@@ -1812,120 +2716,125 @@
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
-      <c r="I62" s="15"/>
+      <c r="I62" s="14"/>
     </row>
     <row r="63" customFormat="false" ht="46.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B63" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="C63" s="33" t="s">
-        <v>82</v>
+      <c r="B63" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C63" s="28" t="s">
+        <v>84</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E63" s="11"/>
       <c r="F63" s="11"/>
       <c r="G63" s="11"/>
       <c r="H63" s="11"/>
-      <c r="I63" s="15"/>
-    </row>
-    <row r="64" customFormat="false" ht="54.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B64" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="C64" s="8" t="s">
+      <c r="I63" s="14"/>
+    </row>
+    <row r="64" customFormat="false" ht="24.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B64" s="27"/>
+      <c r="C64" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="D64" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="14"/>
+    </row>
+    <row r="65" customFormat="false" ht="55.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B65" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D65" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E65" s="26"/>
+      <c r="F65" s="26"/>
+      <c r="G65" s="26"/>
+      <c r="H65" s="26"/>
+      <c r="I65" s="14"/>
+    </row>
+    <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I66" s="14"/>
+    </row>
+    <row r="67" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B67" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C67" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="D64" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="E64" s="30"/>
-      <c r="F64" s="30"/>
-      <c r="G64" s="30"/>
-      <c r="H64" s="30"/>
-      <c r="I64" s="15"/>
-    </row>
-    <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I65" s="15"/>
-    </row>
-    <row r="66" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B66" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="C66" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="E66" s="11"/>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
-      <c r="I66" s="15"/>
-    </row>
-    <row r="67" customFormat="false" ht="55.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B67" s="32"/>
-      <c r="C67" s="12" t="s">
-        <v>86</v>
-      </c>
       <c r="D67" s="11" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="E67" s="11"/>
       <c r="F67" s="11"/>
       <c r="G67" s="11"/>
       <c r="H67" s="11"/>
-      <c r="I67" s="15"/>
-    </row>
-    <row r="68" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="32" t="s">
-        <v>87</v>
-      </c>
-      <c r="C68" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="D68" s="30" t="s">
+      <c r="I67" s="14"/>
+    </row>
+    <row r="68" customFormat="false" ht="55.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B68" s="27"/>
+      <c r="C68" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D68" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11"/>
+      <c r="I68" s="14"/>
+    </row>
+    <row r="69" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C69" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D69" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="E68" s="30"/>
-      <c r="F68" s="30"/>
-      <c r="G68" s="30"/>
-      <c r="H68" s="30"/>
-      <c r="I68" s="15"/>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="35"/>
-      <c r="C69" s="8"/>
-      <c r="D69" s="9"/>
-      <c r="E69" s="9"/>
-      <c r="F69" s="9"/>
-      <c r="G69" s="9"/>
-      <c r="H69" s="9"/>
-      <c r="I69" s="15"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="26"/>
+      <c r="G69" s="26"/>
+      <c r="H69" s="26"/>
+      <c r="I69" s="14"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="35"/>
+      <c r="B70" s="30"/>
       <c r="C70" s="8"/>
       <c r="D70" s="9"/>
       <c r="E70" s="9"/>
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
       <c r="H70" s="9"/>
-      <c r="I70" s="15"/>
+      <c r="I70" s="14"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="35"/>
+      <c r="B71" s="30"/>
       <c r="C71" s="8"/>
       <c r="D71" s="9"/>
       <c r="E71" s="9"/>
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
       <c r="H71" s="9"/>
+      <c r="I71" s="14"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="35"/>
+      <c r="B72" s="30"/>
       <c r="C72" s="8"/>
       <c r="D72" s="9"/>
       <c r="E72" s="9"/>
@@ -1933,17 +2842,18 @@
       <c r="G72" s="9"/>
       <c r="H72" s="9"/>
     </row>
-    <row r="75" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C77" s="36"/>
-      <c r="D77" s="9"/>
-      <c r="E77" s="9"/>
-      <c r="F77" s="9"/>
-      <c r="G77" s="9"/>
-      <c r="H77" s="9"/>
-    </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="35"/>
+    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="30"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
+      <c r="G73" s="9"/>
+      <c r="H73" s="9"/>
+    </row>
+    <row r="76" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C78" s="31"/>
       <c r="D78" s="9"/>
       <c r="E78" s="9"/>
       <c r="F78" s="9"/>
@@ -1951,38 +2861,37 @@
       <c r="H78" s="9"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="35"/>
+      <c r="B79" s="30"/>
       <c r="D79" s="9"/>
       <c r="E79" s="9"/>
       <c r="F79" s="9"/>
       <c r="G79" s="9"/>
       <c r="H79" s="9"/>
     </row>
-    <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B80" s="30"/>
       <c r="D80" s="9"/>
       <c r="E80" s="9"/>
       <c r="F80" s="9"/>
       <c r="G80" s="9"/>
       <c r="H80" s="9"/>
     </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="35"/>
+    <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D81" s="9"/>
       <c r="E81" s="9"/>
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
       <c r="H81" s="9"/>
     </row>
-    <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C82" s="8"/>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B82" s="30"/>
       <c r="D82" s="9"/>
       <c r="E82" s="9"/>
       <c r="F82" s="9"/>
       <c r="G82" s="9"/>
       <c r="H82" s="9"/>
     </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="35"/>
+    <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C83" s="8"/>
       <c r="D83" s="9"/>
       <c r="E83" s="9"/>
@@ -1991,7 +2900,7 @@
       <c r="H83" s="9"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="35"/>
+      <c r="B84" s="30"/>
       <c r="C84" s="8"/>
       <c r="D84" s="9"/>
       <c r="E84" s="9"/>
@@ -2000,7 +2909,7 @@
       <c r="H84" s="9"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="37"/>
+      <c r="B85" s="30"/>
       <c r="C85" s="8"/>
       <c r="D85" s="9"/>
       <c r="E85" s="9"/>
@@ -2009,7 +2918,7 @@
       <c r="H85" s="9"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="35"/>
+      <c r="B86" s="32"/>
       <c r="C86" s="8"/>
       <c r="D86" s="9"/>
       <c r="E86" s="9"/>
@@ -2018,7 +2927,7 @@
       <c r="H86" s="9"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="35"/>
+      <c r="B87" s="30"/>
       <c r="C87" s="8"/>
       <c r="D87" s="9"/>
       <c r="E87" s="9"/>
@@ -2027,7 +2936,7 @@
       <c r="H87" s="9"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="35"/>
+      <c r="B88" s="30"/>
       <c r="C88" s="8"/>
       <c r="D88" s="9"/>
       <c r="E88" s="9"/>
@@ -2036,7 +2945,7 @@
       <c r="H88" s="9"/>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="35"/>
+      <c r="B89" s="30"/>
       <c r="C89" s="8"/>
       <c r="D89" s="9"/>
       <c r="E89" s="9"/>
@@ -2045,7 +2954,7 @@
       <c r="H89" s="9"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="37"/>
+      <c r="B90" s="30"/>
       <c r="C90" s="8"/>
       <c r="D90" s="9"/>
       <c r="E90" s="9"/>
@@ -2054,7 +2963,7 @@
       <c r="H90" s="9"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="35"/>
+      <c r="B91" s="32"/>
       <c r="C91" s="8"/>
       <c r="D91" s="9"/>
       <c r="E91" s="9"/>
@@ -2063,7 +2972,7 @@
       <c r="H91" s="9"/>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="35"/>
+      <c r="B92" s="30"/>
       <c r="C92" s="8"/>
       <c r="D92" s="9"/>
       <c r="E92" s="9"/>
@@ -2072,8 +2981,8 @@
       <c r="H92" s="9"/>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="35"/>
-      <c r="C93" s="36"/>
+      <c r="B93" s="30"/>
+      <c r="C93" s="8"/>
       <c r="D93" s="9"/>
       <c r="E93" s="9"/>
       <c r="F93" s="9"/>
@@ -2081,8 +2990,8 @@
       <c r="H93" s="9"/>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="35"/>
-      <c r="C94" s="36"/>
+      <c r="B94" s="30"/>
+      <c r="C94" s="31"/>
       <c r="D94" s="9"/>
       <c r="E94" s="9"/>
       <c r="F94" s="9"/>
@@ -2090,8 +2999,8 @@
       <c r="H94" s="9"/>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="35"/>
-      <c r="C95" s="36"/>
+      <c r="B95" s="30"/>
+      <c r="C95" s="31"/>
       <c r="D95" s="9"/>
       <c r="E95" s="9"/>
       <c r="F95" s="9"/>
@@ -2099,8 +3008,8 @@
       <c r="H95" s="9"/>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="35"/>
-      <c r="C96" s="36"/>
+      <c r="B96" s="30"/>
+      <c r="C96" s="31"/>
       <c r="D96" s="9"/>
       <c r="E96" s="9"/>
       <c r="F96" s="9"/>
@@ -2108,8 +3017,8 @@
       <c r="H96" s="9"/>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="35"/>
-      <c r="C97" s="36"/>
+      <c r="B97" s="30"/>
+      <c r="C97" s="31"/>
       <c r="D97" s="9"/>
       <c r="E97" s="9"/>
       <c r="F97" s="9"/>
@@ -2117,8 +3026,8 @@
       <c r="H97" s="9"/>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="35"/>
-      <c r="C98" s="36"/>
+      <c r="B98" s="30"/>
+      <c r="C98" s="31"/>
       <c r="D98" s="9"/>
       <c r="E98" s="9"/>
       <c r="F98" s="9"/>
@@ -2126,7 +3035,8 @@
       <c r="H98" s="9"/>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="35"/>
+      <c r="B99" s="30"/>
+      <c r="C99" s="31"/>
       <c r="D99" s="9"/>
       <c r="E99" s="9"/>
       <c r="F99" s="9"/>
@@ -2134,7 +3044,7 @@
       <c r="H99" s="9"/>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="35"/>
+      <c r="B100" s="30"/>
       <c r="D100" s="9"/>
       <c r="E100" s="9"/>
       <c r="F100" s="9"/>
@@ -2142,7 +3052,7 @@
       <c r="H100" s="9"/>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="35"/>
+      <c r="B101" s="30"/>
       <c r="D101" s="9"/>
       <c r="E101" s="9"/>
       <c r="F101" s="9"/>
@@ -2150,7 +3060,7 @@
       <c r="H101" s="9"/>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="38"/>
+      <c r="B102" s="30"/>
       <c r="D102" s="9"/>
       <c r="E102" s="9"/>
       <c r="F102" s="9"/>
@@ -2158,7 +3068,7 @@
       <c r="H102" s="9"/>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="38"/>
+      <c r="B103" s="33"/>
       <c r="D103" s="9"/>
       <c r="E103" s="9"/>
       <c r="F103" s="9"/>
@@ -2166,7 +3076,7 @@
       <c r="H103" s="9"/>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="38"/>
+      <c r="B104" s="33"/>
       <c r="D104" s="9"/>
       <c r="E104" s="9"/>
       <c r="F104" s="9"/>
@@ -2174,7 +3084,7 @@
       <c r="H104" s="9"/>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="38"/>
+      <c r="B105" s="33"/>
       <c r="D105" s="9"/>
       <c r="E105" s="9"/>
       <c r="F105" s="9"/>
@@ -2182,7 +3092,7 @@
       <c r="H105" s="9"/>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B106" s="38"/>
+      <c r="B106" s="33"/>
       <c r="D106" s="9"/>
       <c r="E106" s="9"/>
       <c r="F106" s="9"/>
@@ -2190,7 +3100,7 @@
       <c r="H106" s="9"/>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="38"/>
+      <c r="B107" s="33"/>
       <c r="D107" s="9"/>
       <c r="E107" s="9"/>
       <c r="F107" s="9"/>
@@ -2198,7 +3108,7 @@
       <c r="H107" s="9"/>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="38"/>
+      <c r="B108" s="33"/>
       <c r="D108" s="9"/>
       <c r="E108" s="9"/>
       <c r="F108" s="9"/>
@@ -2206,7 +3116,7 @@
       <c r="H108" s="9"/>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B109" s="38"/>
+      <c r="B109" s="33"/>
       <c r="D109" s="9"/>
       <c r="E109" s="9"/>
       <c r="F109" s="9"/>
@@ -2214,7 +3124,7 @@
       <c r="H109" s="9"/>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="38"/>
+      <c r="B110" s="33"/>
       <c r="D110" s="9"/>
       <c r="E110" s="9"/>
       <c r="F110" s="9"/>
@@ -2222,7 +3132,7 @@
       <c r="H110" s="9"/>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B111" s="38"/>
+      <c r="B111" s="33"/>
       <c r="D111" s="9"/>
       <c r="E111" s="9"/>
       <c r="F111" s="9"/>
@@ -2230,14 +3140,15 @@
       <c r="H111" s="9"/>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B112" s="38"/>
+      <c r="B112" s="33"/>
       <c r="D112" s="9"/>
       <c r="E112" s="9"/>
       <c r="F112" s="9"/>
       <c r="G112" s="9"/>
       <c r="H112" s="9"/>
     </row>
-    <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B113" s="33"/>
       <c r="D113" s="9"/>
       <c r="E113" s="9"/>
       <c r="F113" s="9"/>
@@ -2755,8 +3666,15 @@
       <c r="G186" s="9"/>
       <c r="H186" s="9"/>
     </row>
+    <row r="187" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D187" s="9"/>
+      <c r="E187" s="9"/>
+      <c r="F187" s="9"/>
+      <c r="G187" s="9"/>
+      <c r="H187" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="189">
+  <mergeCells count="191">
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:M2"/>
     <mergeCell ref="B3:H3"/>
@@ -2829,6 +3747,7 @@
     <mergeCell ref="D62:H62"/>
     <mergeCell ref="D63:H63"/>
     <mergeCell ref="D64:H64"/>
+    <mergeCell ref="D65:H65"/>
     <mergeCell ref="D66:H66"/>
     <mergeCell ref="D67:H67"/>
     <mergeCell ref="D68:H68"/>
@@ -2836,7 +3755,7 @@
     <mergeCell ref="D70:H70"/>
     <mergeCell ref="D71:H71"/>
     <mergeCell ref="D72:H72"/>
-    <mergeCell ref="D77:H77"/>
+    <mergeCell ref="D73:H73"/>
     <mergeCell ref="D78:H78"/>
     <mergeCell ref="D79:H79"/>
     <mergeCell ref="D80:H80"/>
@@ -2946,6 +3865,7 @@
     <mergeCell ref="D184:H184"/>
     <mergeCell ref="D185:H185"/>
     <mergeCell ref="D186:H186"/>
+    <mergeCell ref="D187:H187"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>